<commit_message>
SkinNameService called only once per Skin
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="872">
   <si>
     <t>Aatrox</t>
   </si>
@@ -3301,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J149" sqref="J149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3473,7 +3473,9 @@
       <c r="P6" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="3" t="s">
+        <v>282</v>
+      </c>
       <c r="R6" s="2"/>
       <c r="U6" s="17"/>
     </row>
@@ -4920,6 +4922,9 @@
       <c r="K44" s="11" t="s">
         <v>407</v>
       </c>
+      <c r="L44" s="1" t="s">
+        <v>282</v>
+      </c>
       <c r="Q44" s="3"/>
       <c r="R44" s="2"/>
     </row>
@@ -6877,6 +6882,9 @@
       <c r="H98" s="11" t="s">
         <v>174</v>
       </c>
+      <c r="I98" s="1" t="s">
+        <v>282</v>
+      </c>
       <c r="Q98" s="3"/>
       <c r="R98" s="2"/>
     </row>
@@ -7151,6 +7159,9 @@
       </c>
       <c r="N106" s="12" t="s">
         <v>427</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="Q106" s="3"/>
       <c r="R106" s="2"/>
@@ -8610,6 +8621,9 @@
       </c>
       <c r="I149" s="1" t="s">
         <v>857</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="Q149" s="3"/>
       <c r="R149" s="2"/>

</xml_diff>

<commit_message>
Patch 12.15 and 12.16
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="894">
   <si>
     <t>Aatrox</t>
   </si>
@@ -2694,6 +2694,27 @@
   </si>
   <si>
     <t>Nilah</t>
+  </si>
+  <si>
+    <t>Monster Tamer</t>
+  </si>
+  <si>
+    <t>Zap'Maw</t>
+  </si>
+  <si>
+    <t>Cyber Halo</t>
+  </si>
+  <si>
+    <t>Prestige Cyber Halo</t>
+  </si>
+  <si>
+    <t>Armored Titan</t>
+  </si>
+  <si>
+    <t>Strike Commander</t>
+  </si>
+  <si>
+    <t>Strike Paladin</t>
   </si>
 </sst>
 </file>
@@ -3346,8 +3367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M126" sqref="M126"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4155,6 +4176,9 @@
       <c r="F23" s="9" t="s">
         <v>279</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>892</v>
+      </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="2"/>
     </row>
@@ -5182,6 +5206,12 @@
       <c r="N50" s="1" t="s">
         <v>677</v>
       </c>
+      <c r="O50" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>890</v>
+      </c>
       <c r="Q50" s="3"/>
       <c r="R50" s="2"/>
     </row>
@@ -5832,6 +5862,9 @@
       <c r="N68" s="7" t="s">
         <v>485</v>
       </c>
+      <c r="O68" s="1" t="s">
+        <v>888</v>
+      </c>
       <c r="Q68" s="3"/>
       <c r="R68" s="2"/>
     </row>
@@ -6060,6 +6093,9 @@
       <c r="L74" s="7" t="s">
         <v>279</v>
       </c>
+      <c r="M74" s="1" t="s">
+        <v>893</v>
+      </c>
       <c r="Q74" s="3"/>
       <c r="R74" s="2"/>
     </row>
@@ -6100,6 +6136,9 @@
       <c r="L75" s="14" t="s">
         <v>865</v>
       </c>
+      <c r="M75" s="1" t="s">
+        <v>887</v>
+      </c>
       <c r="Q75" s="3"/>
       <c r="R75" s="2"/>
     </row>
@@ -6543,6 +6582,9 @@
       </c>
       <c r="L85" s="13" t="s">
         <v>253</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>891</v>
       </c>
       <c r="Q85" s="3"/>
       <c r="R85" s="2"/>
@@ -8357,22 +8399,22 @@
       <c r="A138" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B138" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C138" s="14" t="s">
+      <c r="B138" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C138" s="17" t="s">
         <v>719</v>
       </c>
-      <c r="D138" s="12" t="s">
+      <c r="D138" s="17" t="s">
         <v>720</v>
       </c>
       <c r="E138" s="11" t="s">
         <v>721</v>
       </c>
-      <c r="F138" s="12" t="s">
+      <c r="F138" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="G138" s="12" t="s">
+      <c r="G138" s="17" t="s">
         <v>722</v>
       </c>
       <c r="Q138" s="3"/>
@@ -8540,6 +8582,9 @@
       </c>
       <c r="N142" s="12" t="s">
         <v>241</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>887</v>
       </c>
       <c r="Q142" s="3"/>
       <c r="R142" s="2"/>

</xml_diff>

<commit_message>
Ratings Skin year 2023
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11805"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2892,10 +2892,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3079,7 +3085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3195,22 +3201,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3227,16 +3230,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF7030A0"/>
       <color rgb="FFFFCC00"/>
-      <color rgb="FFFF9933"/>
-      <color rgb="FF00CC66"/>
-      <color rgb="FF66FF33"/>
+      <color rgb="FF0099CC"/>
       <color rgb="FFCCFF33"/>
       <color rgb="FF00FFCC"/>
-      <color rgb="FF0099CC"/>
-      <color rgb="FF3333FF"/>
-      <color rgb="FF666699"/>
+      <color rgb="FF66FF33"/>
+      <color rgb="FF00CC66"/>
+      <color rgb="FFFF9933"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFFC000"/>
+      <color rgb="FF7030A0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3549,8 +3552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,36 +3608,33 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
       <c r="S3" s="3"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
       <c r="R4" s="38"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="43"/>
+      <c r="T4" s="39"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -3667,15 +3667,14 @@
       <c r="J5" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="6" t="s">
         <v>923</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="9" t="s">
         <v>924</v>
       </c>
       <c r="Q5" s="37"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="43"/>
+      <c r="T5" s="39"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -3729,10 +3728,9 @@
       <c r="Q6" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="6" t="s">
         <v>883</v>
       </c>
-      <c r="S6" s="41"/>
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -3787,13 +3785,13 @@
       <c r="Q7" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="9" t="s">
         <v>923</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T7" s="40" t="s">
         <v>861</v>
       </c>
     </row>
@@ -3810,10 +3808,9 @@
       <c r="D8" s="11" t="s">
         <v>677</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>916</v>
       </c>
-      <c r="S8" s="41"/>
       <c r="T8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -3865,7 +3862,6 @@
       <c r="P9" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="S9" s="41"/>
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3911,10 +3907,9 @@
       <c r="N10" s="11" t="s">
         <v>826</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="S10" s="41"/>
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -3957,10 +3952,9 @@
       <c r="M11" s="11" t="s">
         <v>897</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="S11" s="41"/>
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -4015,10 +4009,9 @@
       <c r="Q12" s="7" t="s">
         <v>895</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="8" t="s">
         <v>901</v>
       </c>
-      <c r="S12" s="41"/>
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -4040,10 +4033,9 @@
       <c r="F13" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="13" t="s">
         <v>941</v>
       </c>
-      <c r="S13" s="41"/>
       <c r="T13" s="2"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -4098,10 +4090,10 @@
       <c r="Q14" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="6" t="s">
         <v>923</v>
       </c>
-      <c r="S14" s="41" t="s">
+      <c r="S14" s="6" t="s">
         <v>925</v>
       </c>
       <c r="T14" s="2"/>
@@ -4122,10 +4114,9 @@
       <c r="E15" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="10" t="s">
         <v>921</v>
       </c>
-      <c r="S15" s="41"/>
       <c r="T15" s="2"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -4153,7 +4144,6 @@
       <c r="H16" s="10" t="s">
         <v>896</v>
       </c>
-      <c r="S16" s="41"/>
       <c r="T16" s="2"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -4178,10 +4168,9 @@
       <c r="G17" s="11" t="s">
         <v>824</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="S17" s="41"/>
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -4194,10 +4183,9 @@
       <c r="C18" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="10" t="s">
         <v>931</v>
       </c>
-      <c r="S18" s="41"/>
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -4249,10 +4237,9 @@
       <c r="P19" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="9" t="s">
         <v>944</v>
       </c>
-      <c r="S19" s="41"/>
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -4292,10 +4279,9 @@
       <c r="L20" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="13" t="s">
         <v>936</v>
       </c>
-      <c r="S20" s="41"/>
       <c r="T20" s="2"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -4326,26 +4312,18 @@
       <c r="I21" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="S21" s="41"/>
       <c r="T21" s="2"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>935</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="39" t="s">
+      <c r="B22" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>936</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="S22" s="41"/>
       <c r="T22" s="2"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -4397,13 +4375,12 @@
       <c r="P23" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" s="8" t="s">
         <v>907</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="R23" s="10" t="s">
         <v>923</v>
       </c>
-      <c r="S23" s="41"/>
       <c r="T23" s="2"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -4428,13 +4405,12 @@
       <c r="G24" s="10" t="s">
         <v>891</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="11" t="s">
         <v>901</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="8" t="s">
         <v>902</v>
       </c>
-      <c r="S24" s="41"/>
       <c r="T24" s="2"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -4468,7 +4444,6 @@
       <c r="J25" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="S25" s="41"/>
       <c r="T25" s="2"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -4502,10 +4477,9 @@
       <c r="J26" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K26" s="6" t="s">
         <v>909</v>
       </c>
-      <c r="S26" s="41"/>
       <c r="T26" s="2"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -4545,7 +4519,6 @@
       <c r="L27" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="S27" s="41"/>
       <c r="T27" s="2"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -4588,7 +4561,6 @@
       <c r="M28" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="S28" s="41"/>
       <c r="T28" s="2"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -4631,7 +4603,6 @@
       <c r="M29" s="7" t="s">
         <v>901</v>
       </c>
-      <c r="S29" s="41"/>
       <c r="T29" s="2"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -4674,10 +4645,9 @@
       <c r="M30" s="11" t="s">
         <v>895</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="N30" s="11" t="s">
         <v>937</v>
       </c>
-      <c r="S30" s="41"/>
       <c r="T30" s="2"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -4717,10 +4687,9 @@
       <c r="L31" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="M31" s="39" t="s">
+      <c r="M31" s="13" t="s">
         <v>936</v>
       </c>
-      <c r="S31" s="41"/>
       <c r="T31" s="2"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -4760,10 +4729,9 @@
       <c r="L32" s="10" t="s">
         <v>868</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M32" s="10" t="s">
         <v>943</v>
       </c>
-      <c r="S32" s="41"/>
       <c r="T32" s="2"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -4794,10 +4762,9 @@
       <c r="I33" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J33" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="S33" s="41"/>
       <c r="T33" s="2"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -4840,10 +4807,9 @@
       <c r="M34" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="N34" s="13" t="s">
         <v>926</v>
       </c>
-      <c r="S34" s="41"/>
       <c r="T34" s="2"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -4904,7 +4870,7 @@
       <c r="S35" s="41" t="s">
         <v>912</v>
       </c>
-      <c r="T35" s="2" t="s">
+      <c r="T35" s="42" t="s">
         <v>941</v>
       </c>
     </row>
@@ -4945,7 +4911,6 @@
       <c r="L36" s="10" t="s">
         <v>884</v>
       </c>
-      <c r="S36" s="41"/>
       <c r="T36" s="2"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -4991,13 +4956,12 @@
       <c r="N37" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="O37" s="8" t="s">
         <v>912</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="P37" s="9" t="s">
         <v>948</v>
       </c>
-      <c r="S37" s="41"/>
       <c r="T37" s="2"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -5037,10 +5001,9 @@
       <c r="L38" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="M38" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="S38" s="41"/>
       <c r="T38" s="2"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -5077,7 +5040,6 @@
       <c r="K39" s="9" t="s">
         <v>904</v>
       </c>
-      <c r="S39" s="41"/>
       <c r="T39" s="2"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -5120,7 +5082,6 @@
       <c r="M40" s="10" t="s">
         <v>841</v>
       </c>
-      <c r="S40" s="41"/>
       <c r="T40" s="2"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -5172,7 +5133,6 @@
       <c r="P41" s="6" t="s">
         <v>904</v>
       </c>
-      <c r="S41" s="41"/>
       <c r="T41" s="2"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -5206,10 +5166,9 @@
       <c r="J42" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="K42" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="S42" s="41"/>
       <c r="T42" s="2"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -5255,7 +5214,6 @@
       <c r="N43" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S43" s="41"/>
       <c r="T43" s="2"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -5301,7 +5259,6 @@
       <c r="N44" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="S44" s="41"/>
       <c r="T44" s="2"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -5317,17 +5274,16 @@
       <c r="D45" s="10" t="s">
         <v>824</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="S45" s="41"/>
       <c r="T45" s="2"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C46" s="13" t="s">
@@ -5360,10 +5316,9 @@
       <c r="L46" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="M46" s="6" t="s">
         <v>901</v>
       </c>
-      <c r="S46" s="41"/>
       <c r="T46" s="2"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -5397,27 +5352,18 @@
       <c r="J47" s="13" t="s">
         <v>832</v>
       </c>
-      <c r="S47" s="41"/>
       <c r="T47" s="2"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B48" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="39" t="s">
+      <c r="B48" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="S48" s="41"/>
       <c r="T48" s="2"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
@@ -5439,7 +5385,6 @@
       <c r="F49" s="6" t="s">
         <v>883</v>
       </c>
-      <c r="S49" s="41"/>
       <c r="T49" s="2"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
@@ -5485,7 +5430,6 @@
       <c r="N50" s="7" t="s">
         <v>904</v>
       </c>
-      <c r="S50" s="41"/>
       <c r="T50" s="2"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
@@ -5504,10 +5448,9 @@
       <c r="E51" s="8" t="s">
         <v>807</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="S51" s="41"/>
       <c r="T51" s="2"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
@@ -5559,7 +5502,6 @@
       <c r="P52" s="8" t="s">
         <v>889</v>
       </c>
-      <c r="S52" s="41"/>
       <c r="T52" s="2"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -5605,38 +5547,37 @@
       <c r="N53" s="7" t="s">
         <v>815</v>
       </c>
-      <c r="O53" s="1" t="s">
+      <c r="O53" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="S53" s="41"/>
       <c r="T53" s="2"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" s="39" t="s">
+      <c r="B54" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="E54" s="39" t="s">
+      <c r="E54" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="F54" s="39" t="s">
+      <c r="F54" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="G54" s="39" t="s">
+      <c r="G54" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="H54" s="39" t="s">
+      <c r="H54" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="I54" s="39" t="s">
+      <c r="I54" s="9" t="s">
         <v>425</v>
       </c>
       <c r="J54" s="11" t="s">
@@ -5660,10 +5601,9 @@
       <c r="P54" s="10" t="s">
         <v>899</v>
       </c>
-      <c r="Q54" s="1" t="s">
+      <c r="Q54" s="11" t="s">
         <v>660</v>
       </c>
-      <c r="S54" s="41"/>
       <c r="T54" s="2"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -5697,7 +5637,6 @@
       <c r="J55" s="11" t="s">
         <v>893</v>
       </c>
-      <c r="S55" s="41"/>
       <c r="T55" s="2"/>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -5731,13 +5670,12 @@
       <c r="J56" s="6" t="s">
         <v>899</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="K56" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="L56" s="1" t="s">
+      <c r="L56" s="9" t="s">
         <v>934</v>
       </c>
-      <c r="S56" s="41"/>
       <c r="T56" s="2"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -5780,10 +5718,9 @@
       <c r="M57" s="12" t="s">
         <v>858</v>
       </c>
-      <c r="N57" s="1" t="s">
+      <c r="N57" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="S57" s="41"/>
       <c r="T57" s="2"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
@@ -5820,10 +5757,9 @@
       <c r="K58" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="L58" s="10" t="s">
         <v>921</v>
       </c>
-      <c r="S58" s="41"/>
       <c r="T58" s="2"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
@@ -5845,10 +5781,9 @@
       <c r="F59" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G59" s="6" t="s">
         <v>912</v>
       </c>
-      <c r="S59" s="41"/>
       <c r="T59" s="2"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
@@ -5894,10 +5829,9 @@
       <c r="N60" s="8" t="s">
         <v>820</v>
       </c>
-      <c r="O60" s="1" t="s">
+      <c r="O60" s="6" t="s">
         <v>911</v>
       </c>
-      <c r="S60" s="41"/>
       <c r="T60" s="2"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
@@ -5931,10 +5865,9 @@
       <c r="J61" s="10" t="s">
         <v>812</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="K61" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="S61" s="41"/>
       <c r="T61" s="2"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -5965,13 +5898,12 @@
       <c r="I62" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="J62" s="40" t="s">
+      <c r="J62" s="8" t="s">
         <v>776</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="K62" s="10" t="s">
         <v>948</v>
       </c>
-      <c r="S62" s="41"/>
       <c r="T62" s="2"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
@@ -6023,13 +5955,12 @@
       <c r="P63" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="Q63" s="1" t="s">
+      <c r="Q63" s="6" t="s">
         <v>912</v>
       </c>
-      <c r="R63" s="1" t="s">
+      <c r="R63" s="7" t="s">
         <v>913</v>
       </c>
-      <c r="S63" s="41"/>
       <c r="T63" s="2"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
@@ -6078,10 +6009,9 @@
       <c r="O64" s="6" t="s">
         <v>840</v>
       </c>
-      <c r="P64" s="1" t="s">
+      <c r="P64" s="8" t="s">
         <v>929</v>
       </c>
-      <c r="S64" s="41"/>
       <c r="T64" s="2"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
@@ -6106,10 +6036,9 @@
       <c r="G65" s="7" t="s">
         <v>883</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="13" t="s">
         <v>941</v>
       </c>
-      <c r="S65" s="41"/>
       <c r="T65" s="2"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
@@ -6146,10 +6075,9 @@
       <c r="K66" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="L66" s="1" t="s">
+      <c r="L66" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="S66" s="41"/>
       <c r="T66" s="2"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
@@ -6180,7 +6108,6 @@
       <c r="I67" s="8" t="s">
         <v>557</v>
       </c>
-      <c r="S67" s="41"/>
       <c r="T67" s="2"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
@@ -6202,13 +6129,12 @@
       <c r="F68" s="6" t="s">
         <v>826</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="G68" s="12" t="s">
         <v>920</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H68" s="10" t="s">
         <v>923</v>
       </c>
-      <c r="S68" s="41"/>
       <c r="T68" s="2"/>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
@@ -6227,10 +6153,9 @@
       <c r="E69" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" s="12" t="s">
         <v>919</v>
       </c>
-      <c r="S69" s="41"/>
       <c r="T69" s="2"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
@@ -6279,10 +6204,9 @@
       <c r="O70" s="11" t="s">
         <v>887</v>
       </c>
-      <c r="P70" s="1" t="s">
+      <c r="P70" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="S70" s="41"/>
       <c r="T70" s="2"/>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
@@ -6298,10 +6222,9 @@
       <c r="D71" s="6" t="s">
         <v>900</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="S71" s="41"/>
       <c r="T71" s="2"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
@@ -6347,7 +6270,6 @@
       <c r="N72" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="S72" s="41"/>
       <c r="T72" s="2"/>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
@@ -6399,7 +6321,6 @@
       <c r="P73" s="11" t="s">
         <v>893</v>
       </c>
-      <c r="S73" s="41"/>
       <c r="T73" s="2"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
@@ -6451,10 +6372,9 @@
       <c r="P74" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="Q74" s="1" t="s">
+      <c r="Q74" s="7" t="s">
         <v>925</v>
       </c>
-      <c r="S74" s="41"/>
       <c r="T74" s="2"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
@@ -6470,10 +6390,9 @@
       <c r="D75" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="S75" s="41"/>
       <c r="T75" s="2"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
@@ -6507,7 +6426,6 @@
       <c r="J76" s="7" t="s">
         <v>865</v>
       </c>
-      <c r="S76" s="41"/>
       <c r="T76" s="2"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
@@ -6550,10 +6468,9 @@
       <c r="M77" s="11" t="s">
         <v>892</v>
       </c>
-      <c r="N77" s="1" t="s">
+      <c r="N77" s="8" t="s">
         <v>901</v>
       </c>
-      <c r="S77" s="41"/>
       <c r="T77" s="2"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
@@ -6596,10 +6513,9 @@
       <c r="M78" s="13" t="s">
         <v>886</v>
       </c>
-      <c r="N78" s="1" t="s">
+      <c r="N78" s="11" t="s">
         <v>824</v>
       </c>
-      <c r="S78" s="41"/>
       <c r="T78" s="2"/>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
@@ -6657,7 +6573,7 @@
       <c r="R79" s="8" t="s">
         <v>865</v>
       </c>
-      <c r="S79" s="42" t="s">
+      <c r="S79" s="9" t="s">
         <v>899</v>
       </c>
       <c r="T79" s="2"/>
@@ -6708,7 +6624,6 @@
       <c r="O80" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="S80" s="41"/>
       <c r="T80" s="2"/>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
@@ -6748,10 +6663,9 @@
       <c r="L81" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="M81" s="8" t="s">
         <v>916</v>
       </c>
-      <c r="S81" s="41"/>
       <c r="T81" s="2"/>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
@@ -6788,10 +6702,9 @@
       <c r="K82" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="L82" s="1" t="s">
+      <c r="L82" s="11" t="s">
         <v>923</v>
       </c>
-      <c r="S82" s="41"/>
       <c r="T82" s="2"/>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
@@ -6843,36 +6756,21 @@
       <c r="P83" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="Q83" s="1" t="s">
+      <c r="Q83" s="10" t="s">
         <v>921</v>
       </c>
-      <c r="S83" s="41"/>
       <c r="T83" s="2"/>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>915</v>
       </c>
-      <c r="B84" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C84" s="39" t="s">
+      <c r="B84" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="11" t="s">
         <v>912</v>
       </c>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="39"/>
-      <c r="I84" s="39"/>
-      <c r="J84" s="39"/>
-      <c r="K84" s="39"/>
-      <c r="L84" s="39"/>
-      <c r="M84" s="39"/>
-      <c r="N84" s="39"/>
-      <c r="O84" s="39"/>
-      <c r="P84" s="39"/>
-      <c r="S84" s="41"/>
       <c r="T84" s="2"/>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
@@ -6930,10 +6828,10 @@
       <c r="R85" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="S85" s="41" t="s">
+      <c r="S85" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="T85" s="2" t="s">
+      <c r="T85" s="43" t="s">
         <v>910</v>
       </c>
     </row>
@@ -6974,10 +6872,9 @@
       <c r="L86" s="6" t="s">
         <v>903</v>
       </c>
-      <c r="M86" s="1" t="s">
+      <c r="M86" s="11" t="s">
         <v>807</v>
       </c>
-      <c r="S86" s="41"/>
       <c r="T86" s="2"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
@@ -7026,35 +6923,21 @@
       <c r="O87" s="8" t="s">
         <v>884</v>
       </c>
-      <c r="P87" s="1" t="s">
+      <c r="P87" s="7" t="s">
         <v>883</v>
       </c>
-      <c r="S87" s="41"/>
       <c r="T87" s="2"/>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>927</v>
       </c>
-      <c r="B88" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C88" s="39" t="s">
+      <c r="B88" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>926</v>
       </c>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
-      <c r="F88" s="39"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="39"/>
-      <c r="I88" s="39"/>
-      <c r="J88" s="39"/>
-      <c r="K88" s="39"/>
-      <c r="L88" s="39"/>
-      <c r="M88" s="39"/>
-      <c r="N88" s="39"/>
-      <c r="O88" s="39"/>
-      <c r="S88" s="41"/>
       <c r="T88" s="2"/>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
@@ -7097,10 +6980,9 @@
       <c r="M89" s="6" t="s">
         <v>864</v>
       </c>
-      <c r="N89" s="1" t="s">
+      <c r="N89" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="S89" s="41"/>
       <c r="T89" s="2"/>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
@@ -7143,10 +7025,9 @@
       <c r="M90" s="10" t="s">
         <v>890</v>
       </c>
-      <c r="N90" s="1" t="s">
+      <c r="N90" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="S90" s="41"/>
       <c r="T90" s="2"/>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
@@ -7180,10 +7061,9 @@
       <c r="J91" s="6" t="s">
         <v>895</v>
       </c>
-      <c r="K91" s="1" t="s">
+      <c r="K91" s="6" t="s">
         <v>932</v>
       </c>
-      <c r="S91" s="41"/>
       <c r="T91" s="2"/>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
@@ -7208,10 +7088,9 @@
       <c r="G92" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="H92" s="39" t="s">
+      <c r="H92" s="12" t="s">
         <v>936</v>
       </c>
-      <c r="S92" s="41"/>
       <c r="T92" s="2"/>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
@@ -7260,13 +7139,12 @@
       <c r="O93" s="11" t="s">
         <v>881</v>
       </c>
-      <c r="P93" s="1" t="s">
+      <c r="P93" s="13" t="s">
         <v>917</v>
       </c>
-      <c r="Q93" s="1" t="s">
+      <c r="Q93" s="8" t="s">
         <v>937</v>
       </c>
-      <c r="S93" s="41"/>
       <c r="T93" s="2"/>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
@@ -7279,10 +7157,9 @@
       <c r="C94" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="S94" s="41"/>
       <c r="T94" s="2"/>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
@@ -7316,10 +7193,9 @@
       <c r="J95" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="K95" s="1" t="s">
+      <c r="K95" s="6" t="s">
         <v>909</v>
       </c>
-      <c r="S95" s="41"/>
       <c r="T95" s="2"/>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
@@ -7359,10 +7235,9 @@
       <c r="L96" s="10" t="s">
         <v>834</v>
       </c>
-      <c r="M96" s="1" t="s">
+      <c r="M96" s="10" t="s">
         <v>933</v>
       </c>
-      <c r="S96" s="41"/>
       <c r="T96" s="2"/>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
@@ -7402,7 +7277,6 @@
       <c r="L97" s="13" t="s">
         <v>812</v>
       </c>
-      <c r="S97" s="41"/>
       <c r="T97" s="2"/>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
@@ -7442,10 +7316,9 @@
       <c r="L98" s="8" t="s">
         <v>831</v>
       </c>
-      <c r="M98" s="1" t="s">
+      <c r="M98" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="S98" s="41"/>
       <c r="T98" s="2"/>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
@@ -7464,7 +7337,6 @@
       <c r="E99" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="S99" s="41"/>
       <c r="T99" s="2"/>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
@@ -7510,7 +7382,6 @@
       <c r="N100" s="10" t="s">
         <v>839</v>
       </c>
-      <c r="S100" s="41"/>
       <c r="T100" s="2"/>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
@@ -7553,10 +7424,9 @@
       <c r="M101" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="N101" s="1" t="s">
+      <c r="N101" s="10" t="s">
         <v>824</v>
       </c>
-      <c r="S101" s="41"/>
       <c r="T101" s="2"/>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
@@ -7587,13 +7457,12 @@
       <c r="I102" s="6" t="s">
         <v>899</v>
       </c>
-      <c r="J102" s="1" t="s">
+      <c r="J102" s="13" t="s">
         <v>926</v>
       </c>
-      <c r="K102" s="1" t="s">
+      <c r="K102" s="11" t="s">
         <v>928</v>
       </c>
-      <c r="S102" s="41"/>
       <c r="T102" s="2"/>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
@@ -7621,10 +7490,9 @@
       <c r="H103" s="7" t="s">
         <v>510</v>
       </c>
-      <c r="I103" s="1" t="s">
+      <c r="I103" s="8" t="s">
         <v>937</v>
       </c>
-      <c r="S103" s="41"/>
       <c r="T103" s="2"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
@@ -7652,7 +7520,6 @@
       <c r="H104" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="S104" s="41"/>
       <c r="T104" s="2"/>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
@@ -7683,19 +7550,18 @@
       <c r="I105" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="J105" s="1" t="s">
+      <c r="J105" s="6" t="s">
         <v>909</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="K105" s="6" t="s">
         <v>940</v>
       </c>
-      <c r="L105" s="1" t="s">
+      <c r="L105" s="9" t="s">
         <v>948</v>
       </c>
-      <c r="M105" s="1" t="s">
+      <c r="M105" s="10" t="s">
         <v>949</v>
       </c>
-      <c r="S105" s="41"/>
       <c r="T105" s="2"/>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
@@ -7735,7 +7601,6 @@
       <c r="L106" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="S106" s="41"/>
       <c r="T106" s="2"/>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
@@ -7757,7 +7622,6 @@
       <c r="F107" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="S107" s="41"/>
       <c r="T107" s="2"/>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
@@ -7773,7 +7637,6 @@
       <c r="D108" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="S108" s="41"/>
       <c r="T108" s="2"/>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
@@ -7789,13 +7652,12 @@
       <c r="D109" s="6" t="s">
         <v>895</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E109" s="7" t="s">
         <v>937</v>
       </c>
-      <c r="F109" s="1" t="s">
+      <c r="F109" s="10" t="s">
         <v>938</v>
       </c>
-      <c r="S109" s="41"/>
       <c r="T109" s="2"/>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
@@ -7841,13 +7703,12 @@
       <c r="N110" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="O110" s="1" t="s">
+      <c r="O110" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="P110" s="1" t="s">
+      <c r="P110" s="6" t="s">
         <v>939</v>
       </c>
-      <c r="S110" s="41"/>
       <c r="T110" s="2"/>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
@@ -7878,10 +7739,9 @@
       <c r="I111" s="8" t="s">
         <v>804</v>
       </c>
-      <c r="J111" s="39" t="s">
+      <c r="J111" s="10" t="s">
         <v>936</v>
       </c>
-      <c r="S111" s="41"/>
       <c r="T111" s="2"/>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
@@ -7933,13 +7793,12 @@
       <c r="P112" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="Q112" s="1" t="s">
+      <c r="Q112" s="9" t="s">
         <v>909</v>
       </c>
-      <c r="R112" s="1" t="s">
+      <c r="R112" s="8" t="s">
         <v>950</v>
       </c>
-      <c r="S112" s="41"/>
       <c r="T112" s="2"/>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
@@ -7964,10 +7823,9 @@
       <c r="G113" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="H113" s="1" t="s">
+      <c r="H113" s="13" t="s">
         <v>824</v>
       </c>
-      <c r="S113" s="41"/>
       <c r="T113" s="2"/>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
@@ -8016,7 +7874,6 @@
       <c r="O114" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="S114" s="41"/>
       <c r="T114" s="2"/>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
@@ -8035,10 +7892,9 @@
       <c r="E115" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F115" s="6" t="s">
         <v>926</v>
       </c>
-      <c r="S115" s="41"/>
       <c r="T115" s="2"/>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
@@ -8084,7 +7940,6 @@
       <c r="N116" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="S116" s="41"/>
       <c r="T116" s="2"/>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
@@ -8115,13 +7970,12 @@
       <c r="I117" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="J117" s="1" t="s">
+      <c r="J117" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="K117" s="1" t="s">
+      <c r="K117" s="8" t="s">
         <v>901</v>
       </c>
-      <c r="S117" s="41"/>
       <c r="T117" s="2"/>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.25">
@@ -8149,13 +8003,12 @@
       <c r="H118" s="8" t="s">
         <v>882</v>
       </c>
-      <c r="I118" s="1" t="s">
+      <c r="I118" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="J118" s="1" t="s">
+      <c r="J118" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="S118" s="41"/>
       <c r="T118" s="2"/>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.25">
@@ -8183,13 +8036,12 @@
       <c r="H119" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="I119" s="1" t="s">
+      <c r="I119" s="10" t="s">
         <v>926</v>
       </c>
-      <c r="J119" s="1" t="s">
+      <c r="J119" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="S119" s="41"/>
       <c r="T119" s="2"/>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
@@ -8232,13 +8084,12 @@
       <c r="M120" s="11" t="s">
         <v>901</v>
       </c>
-      <c r="N120" s="1" t="s">
+      <c r="N120" s="13" t="s">
         <v>926</v>
       </c>
-      <c r="O120" s="1" t="s">
+      <c r="O120" s="13" t="s">
         <v>928</v>
       </c>
-      <c r="S120" s="41"/>
       <c r="T120" s="2"/>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
@@ -8278,10 +8129,9 @@
       <c r="L121" s="9" t="s">
         <v>776</v>
       </c>
-      <c r="M121" s="1" t="s">
+      <c r="M121" s="7" t="s">
         <v>914</v>
       </c>
-      <c r="S121" s="41"/>
       <c r="T121" s="2"/>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
@@ -8312,10 +8162,9 @@
       <c r="I122" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="J122" s="1" t="s">
+      <c r="J122" s="8" t="s">
         <v>929</v>
       </c>
-      <c r="S122" s="41"/>
       <c r="T122" s="2"/>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
@@ -8355,10 +8204,9 @@
       <c r="L123" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="M123" s="1" t="s">
+      <c r="M123" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="S123" s="41"/>
       <c r="T123" s="2"/>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.25">
@@ -8392,17 +8240,16 @@
       <c r="J124" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="K124" s="1" t="s">
+      <c r="K124" s="8" t="s">
         <v>932</v>
       </c>
-      <c r="S124" s="41"/>
       <c r="T124" s="2"/>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B125" s="39" t="s">
+      <c r="B125" s="5" t="s">
         <v>157</v>
       </c>
       <c r="C125" s="14" t="s">
@@ -8453,7 +8300,7 @@
       <c r="R125" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="S125" s="41" t="s">
+      <c r="S125" s="9" t="s">
         <v>950</v>
       </c>
       <c r="T125" s="2"/>
@@ -8480,24 +8327,18 @@
       <c r="G126" s="10" t="s">
         <v>665</v>
       </c>
-      <c r="S126" s="41"/>
       <c r="T126" s="2"/>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>952</v>
       </c>
-      <c r="B127" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C127" s="39" t="s">
+      <c r="B127" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C127" s="9" t="s">
         <v>953</v>
       </c>
-      <c r="D127" s="39"/>
-      <c r="E127" s="39"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
-      <c r="S127" s="41"/>
       <c r="T127" s="2"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
@@ -8540,13 +8381,12 @@
       <c r="M128" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="N128" s="1" t="s">
+      <c r="N128" s="7" t="s">
         <v>929</v>
       </c>
-      <c r="O128" s="1" t="s">
+      <c r="O128" s="7" t="s">
         <v>930</v>
       </c>
-      <c r="S128" s="41"/>
       <c r="T128" s="2"/>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.25">
@@ -8598,10 +8438,9 @@
       <c r="P129" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="Q129" s="1" t="s">
+      <c r="Q129" s="6" t="s">
         <v>929</v>
       </c>
-      <c r="S129" s="41"/>
       <c r="T129" s="2"/>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.25">
@@ -8632,7 +8471,6 @@
       <c r="I130" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="S130" s="41"/>
       <c r="T130" s="2"/>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.25">
@@ -8660,17 +8498,16 @@
       <c r="H131" s="9" t="s">
         <v>894</v>
       </c>
-      <c r="I131" s="1" t="s">
+      <c r="I131" s="13" t="s">
         <v>901</v>
       </c>
-      <c r="S131" s="41"/>
       <c r="T131" s="2"/>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B132" s="39" t="s">
+      <c r="B132" s="6" t="s">
         <v>157</v>
       </c>
       <c r="C132" s="10" t="s">
@@ -8706,10 +8543,9 @@
       <c r="M132" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="N132" s="1" t="s">
+      <c r="N132" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="S132" s="41"/>
       <c r="T132" s="2"/>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.25">
@@ -8734,10 +8570,9 @@
       <c r="G133" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="H133" s="1" t="s">
+      <c r="H133" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="S133" s="41"/>
       <c r="T133" s="2"/>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.25">
@@ -8759,10 +8594,9 @@
       <c r="F134" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="G134" s="9" t="s">
         <v>925</v>
       </c>
-      <c r="S134" s="41"/>
       <c r="T134" s="2"/>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
@@ -8802,10 +8636,9 @@
       <c r="L135" s="6" t="s">
         <v>874</v>
       </c>
-      <c r="M135" s="1" t="s">
+      <c r="M135" s="11" t="s">
         <v>950</v>
       </c>
-      <c r="S135" s="41"/>
       <c r="T135" s="2"/>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
@@ -8833,7 +8666,6 @@
       <c r="H136" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S136" s="41"/>
       <c r="T136" s="2"/>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
@@ -8885,7 +8717,6 @@
       <c r="P137" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S137" s="41"/>
       <c r="T137" s="2"/>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
@@ -8934,10 +8765,9 @@
       <c r="O138" s="8" t="s">
         <v>906</v>
       </c>
-      <c r="P138" s="1" t="s">
+      <c r="P138" s="9" t="s">
         <v>901</v>
       </c>
-      <c r="S138" s="41"/>
       <c r="T138" s="2"/>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.25">
@@ -8989,7 +8819,6 @@
       <c r="P139" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="S139" s="41"/>
       <c r="T139" s="2"/>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.25">
@@ -9020,8 +8849,6 @@
       <c r="I140" s="9" t="s">
         <v>895</v>
       </c>
-      <c r="P140" s="39"/>
-      <c r="S140" s="41"/>
       <c r="T140" s="2"/>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">
@@ -9064,7 +8891,6 @@
       <c r="M141" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="S141" s="41"/>
       <c r="T141" s="2"/>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.25">
@@ -9119,7 +8945,6 @@
       <c r="Q142" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S142" s="41"/>
       <c r="T142" s="2"/>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.25">
@@ -9165,7 +8990,6 @@
       <c r="N143" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="S143" s="41"/>
       <c r="T143" s="2"/>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.25">
@@ -9190,10 +9014,9 @@
       <c r="G144" s="10" t="s">
         <v>722</v>
       </c>
-      <c r="H144" s="1" t="s">
+      <c r="H144" s="10" t="s">
         <v>921</v>
       </c>
-      <c r="S144" s="41"/>
       <c r="T144" s="2"/>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.25">
@@ -9221,7 +9044,6 @@
       <c r="H145" s="10" t="s">
         <v>895</v>
       </c>
-      <c r="S145" s="41"/>
       <c r="T145" s="2"/>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.25">
@@ -9264,10 +9086,9 @@
       <c r="M146" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="N146" s="1" t="s">
+      <c r="N146" s="6" t="s">
         <v>883</v>
       </c>
-      <c r="S146" s="41"/>
       <c r="T146" s="2"/>
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.25">
@@ -9319,13 +9140,12 @@
       <c r="P147" s="12" t="s">
         <v>837</v>
       </c>
-      <c r="Q147" s="1" t="s">
+      <c r="Q147" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="R147" s="1" t="s">
+      <c r="R147" s="8" t="s">
         <v>948</v>
       </c>
-      <c r="S147" s="41"/>
       <c r="T147" s="2"/>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">
@@ -9374,10 +9194,9 @@
       <c r="O148" s="12" t="s">
         <v>886</v>
       </c>
-      <c r="P148" s="1" t="s">
+      <c r="P148" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="S148" s="41"/>
       <c r="T148" s="2"/>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.25">
@@ -9402,10 +9221,9 @@
       <c r="G149" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="H149" s="1" t="s">
+      <c r="H149" s="11" t="s">
         <v>946</v>
       </c>
-      <c r="S149" s="41"/>
       <c r="T149" s="2"/>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.25">
@@ -9421,7 +9239,6 @@
       <c r="D150" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="S150" s="41"/>
       <c r="T150" s="2"/>
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.25">
@@ -9458,13 +9275,12 @@
       <c r="K151" s="9" t="s">
         <v>822</v>
       </c>
-      <c r="L151" s="1" t="s">
+      <c r="L151" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="M151" s="1" t="s">
+      <c r="M151" s="6" t="s">
         <v>950</v>
       </c>
-      <c r="S151" s="41"/>
       <c r="T151" s="2"/>
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.25">
@@ -9486,10 +9302,9 @@
       <c r="F152" s="6" t="s">
         <v>596</v>
       </c>
-      <c r="G152" s="1" t="s">
+      <c r="G152" s="13" t="s">
         <v>926</v>
       </c>
-      <c r="S152" s="41"/>
       <c r="T152" s="2"/>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.25">
@@ -9517,7 +9332,6 @@
       <c r="H153" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="S153" s="41"/>
       <c r="T153" s="2"/>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.25">
@@ -9560,10 +9374,9 @@
       <c r="M154" s="11" t="s">
         <v>824</v>
       </c>
-      <c r="N154" s="1" t="s">
+      <c r="N154" s="10" t="s">
         <v>909</v>
       </c>
-      <c r="S154" s="41"/>
       <c r="T154" s="2"/>
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.25">
@@ -9597,10 +9410,9 @@
       <c r="J155" s="8" t="s">
         <v>877</v>
       </c>
-      <c r="K155" s="1" t="s">
+      <c r="K155" s="6" t="s">
         <v>921</v>
       </c>
-      <c r="S155" s="41"/>
       <c r="T155" s="2"/>
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
@@ -9652,7 +9464,6 @@
       <c r="P156" s="6" t="s">
         <v>902</v>
       </c>
-      <c r="S156" s="41"/>
       <c r="T156" s="2"/>
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.25">
@@ -9683,10 +9494,9 @@
       <c r="I157" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="J157" s="1" t="s">
+      <c r="J157" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="S157" s="41"/>
       <c r="T157" s="2"/>
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.25">
@@ -9720,13 +9530,12 @@
       <c r="J158" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="K158" s="1" t="s">
+      <c r="K158" s="7" t="s">
         <v>909</v>
       </c>
-      <c r="L158" s="1" t="s">
+      <c r="L158" s="7" t="s">
         <v>940</v>
       </c>
-      <c r="S158" s="41"/>
       <c r="T158" s="2"/>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.25">
@@ -9754,10 +9563,9 @@
       <c r="H159" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="I159" s="1" t="s">
+      <c r="I159" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="S159" s="41"/>
       <c r="T159" s="2"/>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
@@ -9797,7 +9605,6 @@
       <c r="L160" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="S160" s="41"/>
       <c r="T160" s="2"/>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.25">
@@ -9843,16 +9650,15 @@
       <c r="N161" s="6" t="s">
         <v>842</v>
       </c>
-      <c r="O161" s="1" t="s">
+      <c r="O161" s="6" t="s">
         <v>921</v>
       </c>
-      <c r="P161" s="1" t="s">
+      <c r="P161" s="10" t="s">
         <v>922</v>
       </c>
-      <c r="Q161" s="1" t="s">
+      <c r="Q161" s="8" t="s">
         <v>951</v>
       </c>
-      <c r="S161" s="41"/>
       <c r="T161" s="2"/>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
@@ -9874,16 +9680,15 @@
       <c r="F162" s="13" t="s">
         <v>881</v>
       </c>
-      <c r="G162" s="1" t="s">
+      <c r="G162" s="10" t="s">
         <v>921</v>
       </c>
-      <c r="H162" s="1" t="s">
+      <c r="H162" s="9" t="s">
         <v>941</v>
       </c>
-      <c r="I162" s="1" t="s">
+      <c r="I162" s="9" t="s">
         <v>942</v>
       </c>
-      <c r="S162" s="41"/>
       <c r="T162" s="2"/>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.25">
@@ -9914,7 +9719,6 @@
       <c r="I163" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="S163" s="41"/>
       <c r="T163" s="2"/>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
@@ -9939,10 +9743,9 @@
       <c r="G164" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="H164" s="1" t="s">
+      <c r="H164" s="13" t="s">
         <v>918</v>
       </c>
-      <c r="S164" s="41"/>
       <c r="T164" s="2"/>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
@@ -9967,7 +9770,6 @@
       <c r="G165" s="10" t="s">
         <v>899</v>
       </c>
-      <c r="S165" s="41"/>
       <c r="T165" s="2"/>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
@@ -10007,10 +9809,9 @@
       <c r="L166" s="10" t="s">
         <v>899</v>
       </c>
-      <c r="M166" s="1" t="s">
+      <c r="M166" s="8" t="s">
         <v>929</v>
       </c>
-      <c r="S166" s="41"/>
       <c r="T166" s="2"/>
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.25">
@@ -10026,10 +9827,9 @@
       <c r="D167" s="13" t="s">
         <v>881</v>
       </c>
-      <c r="E167" s="1" t="s">
+      <c r="E167" s="9" t="s">
         <v>929</v>
       </c>
-      <c r="S167" s="41"/>
       <c r="T167" s="2"/>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
@@ -10069,10 +9869,9 @@
       <c r="L168" s="11" t="s">
         <v>833</v>
       </c>
-      <c r="M168" s="1" t="s">
+      <c r="M168" s="12" t="s">
         <v>937</v>
       </c>
-      <c r="S168" s="41"/>
       <c r="T168" s="2"/>
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.25">
@@ -10103,7 +9902,6 @@
       <c r="I169" s="9" t="s">
         <v>901</v>
       </c>
-      <c r="S169" s="41"/>
       <c r="T169" s="2"/>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.25">
@@ -10134,7 +9932,6 @@
       <c r="I170" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="S170" s="41"/>
       <c r="T170" s="2"/>
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.25">
@@ -10171,7 +9968,7 @@
       <c r="K171" s="18" t="s">
         <v>904</v>
       </c>
-      <c r="L171" s="44" t="s">
+      <c r="L171" s="16" t="s">
         <v>936</v>
       </c>
       <c r="M171" s="3"/>
@@ -10188,5 +9985,6 @@
     <mergeCell ref="B4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Patches 14.20 and 14.21
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="999">
   <si>
     <t>Aatrox</t>
   </si>
@@ -3003,6 +3003,24 @@
   </si>
   <si>
     <t>Worlds 2024</t>
+  </si>
+  <si>
+    <t>Music Fan</t>
+  </si>
+  <si>
+    <t>Cosplayer</t>
+  </si>
+  <si>
+    <t>Esports Fan</t>
+  </si>
+  <si>
+    <t>Genesis Nightbringer</t>
+  </si>
+  <si>
+    <t>Ann-Sivir-Sary</t>
+  </si>
+  <si>
+    <t>Prestige Dark Cosmic</t>
   </si>
 </sst>
 </file>
@@ -3707,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I153" sqref="I153"/>
+    <sheetView tabSelected="1" topLeftCell="B142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K164" sqref="K164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4896,6 +4914,12 @@
       <c r="N30" s="1" t="s">
         <v>951</v>
       </c>
+      <c r="O30" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>998</v>
+      </c>
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
       <c r="V30" s="41"/>
@@ -5577,6 +5601,9 @@
       <c r="O44" s="1" t="s">
         <v>232</v>
       </c>
+      <c r="P44" s="1" t="s">
+        <v>993</v>
+      </c>
       <c r="T44" s="41"/>
       <c r="U44" s="41"/>
       <c r="V44" s="41"/>
@@ -6197,6 +6224,9 @@
       </c>
       <c r="M59" s="1" t="s">
         <v>951</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="T59" s="41"/>
       <c r="U59" s="41"/>
@@ -7697,6 +7727,9 @@
       <c r="H93" s="12" t="s">
         <v>934</v>
       </c>
+      <c r="I93" s="1" t="s">
+        <v>994</v>
+      </c>
       <c r="T93" s="41"/>
       <c r="U93" s="41"/>
       <c r="V93" s="41"/>
@@ -9041,7 +9074,9 @@
       <c r="S126" s="9" t="s">
         <v>948</v>
       </c>
-      <c r="T126" s="41"/>
+      <c r="T126" s="41" t="s">
+        <v>997</v>
+      </c>
       <c r="U126" s="41"/>
       <c r="V126" s="41"/>
       <c r="W126" s="2"/>
@@ -9263,6 +9298,9 @@
       <c r="I132" s="13" t="s">
         <v>899</v>
       </c>
+      <c r="J132" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="T132" s="41"/>
       <c r="U132" s="41"/>
       <c r="V132" s="41"/>
@@ -9644,6 +9682,9 @@
       <c r="I141" s="9" t="s">
         <v>893</v>
       </c>
+      <c r="J141" s="1" t="s">
+        <v>995</v>
+      </c>
       <c r="T141" s="41"/>
       <c r="U141" s="41"/>
       <c r="V141" s="41"/>
@@ -10541,6 +10582,9 @@
       <c r="R162" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="S162" s="1" t="s">
+        <v>996</v>
+      </c>
       <c r="T162" s="41"/>
       <c r="U162" s="41"/>
       <c r="V162" s="41"/>
@@ -10613,6 +10657,9 @@
       <c r="I164" s="10" t="s">
         <v>173</v>
       </c>
+      <c r="J164" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="T164" s="41"/>
       <c r="U164" s="41"/>
       <c r="V164" s="41"/>
@@ -10864,6 +10911,9 @@
       </c>
       <c r="I171" s="10" t="s">
         <v>899</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="T171" s="41"/>
       <c r="U171" s="41"/>

</xml_diff>

<commit_message>
Arcane S1 Skins fixed
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1015">
   <si>
     <t>Aatrox</t>
   </si>
@@ -2486,9 +2486,6 @@
     <t>Duality Dragon</t>
   </si>
   <si>
-    <t>Arcane</t>
-  </si>
-  <si>
     <t>Astronautilus</t>
   </si>
   <si>
@@ -2549,9 +2546,6 @@
     <t>Sea Dog</t>
   </si>
   <si>
-    <t>Firelight</t>
-  </si>
-  <si>
     <t>Renata Glasc</t>
   </si>
   <si>
@@ -3060,6 +3054,21 @@
   </si>
   <si>
     <t>Arcane Last Stand</t>
+  </si>
+  <si>
+    <t>Arcane Enforcer</t>
+  </si>
+  <si>
+    <t>Arcane Firelight</t>
+  </si>
+  <si>
+    <t>Arcane Inventor</t>
+  </si>
+  <si>
+    <t>Arcane Enemy</t>
+  </si>
+  <si>
+    <t>Arcane Undercity</t>
   </si>
 </sst>
 </file>
@@ -3764,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="C130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L153" sqref="L153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3871,7 +3880,7 @@
         <v>161</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>162</v>
@@ -3883,13 +3892,13 @@
         <v>500</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="Q5" s="37"/>
       <c r="T5" s="37"/>
@@ -3932,7 +3941,7 @@
         <v>171</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>172</v>
@@ -3950,13 +3959,13 @@
         <v>278</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="T6" s="41" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="U6" s="41"/>
       <c r="V6" s="41"/>
@@ -3997,7 +4006,7 @@
         <v>171</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>183</v>
@@ -4015,16 +4024,16 @@
         <v>170</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>276</v>
       </c>
       <c r="T7" s="42" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="U7" s="41" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="V7" s="41"/>
       <c r="W7" s="2"/>
@@ -4043,7 +4052,7 @@
         <v>675</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="T8" s="41"/>
       <c r="U8" s="41"/>
@@ -4106,13 +4115,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>157</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
@@ -4173,10 +4182,10 @@
         <v>206</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="T11" s="41"/>
       <c r="U11" s="41"/>
@@ -4221,7 +4230,7 @@
         <v>809</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="N12" s="5" t="s">
         <v>162</v>
@@ -4257,7 +4266,7 @@
         <v>219</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>220</v>
@@ -4278,16 +4287,16 @@
         <v>197</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="T13" s="41"/>
       <c r="U13" s="41"/>
@@ -4308,13 +4317,13 @@
         <v>197</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>173</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="T14" s="41"/>
       <c r="U14" s="41"/>
@@ -4353,7 +4362,7 @@
         <v>183</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>231</v>
@@ -4368,16 +4377,16 @@
         <v>276</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="Q15" s="7" t="s">
         <v>509</v>
       </c>
       <c r="R15" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="S15" s="6" t="s">
         <v>921</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>923</v>
       </c>
       <c r="T15" s="41" t="s">
         <v>177</v>
@@ -4403,10 +4412,10 @@
         <v>235</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="T16" s="41"/>
       <c r="U16" s="41"/>
@@ -4415,7 +4424,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B17" s="45" t="s">
         <v>157</v>
@@ -4454,10 +4463,10 @@
         <v>172</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="T18" s="41"/>
       <c r="U18" s="41"/>
@@ -4484,13 +4493,13 @@
         <v>240</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>430</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="T19" s="41"/>
       <c r="U19" s="41"/>
@@ -4499,7 +4508,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>157</v>
@@ -4508,10 +4517,10 @@
         <v>248</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="T20" s="41"/>
       <c r="U20" s="41"/>
@@ -4565,10 +4574,10 @@
         <v>162</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="T21" s="41"/>
       <c r="U21" s="41"/>
@@ -4610,13 +4619,13 @@
         <v>335</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T22" s="41"/>
       <c r="U22" s="41"/>
@@ -4658,16 +4667,16 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>157</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="T24" s="41"/>
       <c r="U24" s="41"/>
@@ -4712,28 +4721,28 @@
         <v>169</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="N25" s="6" t="s">
         <v>274</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>820</v>
+        <v>1010</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="Q25" s="8" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="R25" s="10" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="T25" s="41" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="U25" s="41"/>
       <c r="V25" s="41"/>
@@ -4759,13 +4768,13 @@
         <v>278</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="T26" s="41"/>
       <c r="U26" s="41"/>
@@ -4840,10 +4849,10 @@
         <v>430</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
@@ -4933,10 +4942,10 @@
         <v>173</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="T30" s="41"/>
       <c r="U30" s="41"/>
@@ -4972,7 +4981,7 @@
         <v>307</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>802</v>
@@ -4981,16 +4990,16 @@
         <v>432</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>429</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="T31" s="41"/>
       <c r="U31" s="41"/>
@@ -5035,10 +5044,10 @@
         <v>335</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="N32" s="11" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="T32" s="41"/>
       <c r="U32" s="41"/>
@@ -5083,7 +5092,7 @@
         <v>322</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="T33" s="41"/>
       <c r="U33" s="41"/>
@@ -5119,19 +5128,19 @@
         <v>272</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>841</v>
+        <v>1011</v>
       </c>
       <c r="K34" s="11" t="s">
         <v>170</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="T34" s="41"/>
       <c r="U34" s="41"/>
@@ -5200,7 +5209,7 @@
         <v>171</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>265</v>
@@ -5215,13 +5224,13 @@
         <v>173</v>
       </c>
       <c r="N36" s="13" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>232</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="T36" s="41"/>
       <c r="U36" s="41"/>
@@ -5278,22 +5287,22 @@
         <v>339</v>
       </c>
       <c r="Q37" s="10" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="R37" s="6" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="S37" s="40" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="T37" s="43" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="U37" s="41" t="s">
+        <v>949</v>
+      </c>
+      <c r="V37" s="41" t="s">
         <v>951</v>
-      </c>
-      <c r="V37" s="41" t="s">
-        <v>953</v>
       </c>
       <c r="W37" s="2"/>
     </row>
@@ -5332,7 +5341,7 @@
         <v>347</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>161</v>
@@ -5380,16 +5389,16 @@
         <v>197</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="N39" s="10" t="s">
         <v>326</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>307</v>
@@ -5431,7 +5440,7 @@
         <v>359</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>360</v>
@@ -5440,7 +5449,7 @@
         <v>240</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="T40" s="41"/>
       <c r="U40" s="41"/>
@@ -5479,7 +5488,7 @@
         <v>365</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="T41" s="41"/>
       <c r="U41" s="41"/>
@@ -5524,7 +5533,7 @@
         <v>373</v>
       </c>
       <c r="M42" s="10" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>183</v>
@@ -5575,16 +5584,16 @@
         <v>312</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O43" s="10" t="s">
         <v>274</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="T43" s="41"/>
       <c r="U43" s="41"/>
@@ -5608,7 +5617,7 @@
         <v>239</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G44" s="11" t="s">
         <v>222</v>
@@ -5623,7 +5632,7 @@
         <v>172</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="T44" s="41"/>
       <c r="U44" s="41"/>
@@ -5677,7 +5686,7 @@
         <v>232</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="T45" s="41"/>
       <c r="U45" s="41"/>
@@ -5725,10 +5734,10 @@
         <v>802</v>
       </c>
       <c r="N46" s="11" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="T46" s="41"/>
       <c r="U46" s="41"/>
@@ -5746,10 +5755,10 @@
         <v>252</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>307</v>
@@ -5797,7 +5806,7 @@
         <v>278</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="T48" s="41"/>
       <c r="U48" s="41"/>
@@ -5833,10 +5842,10 @@
         <v>273</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="T49" s="41"/>
       <c r="U49" s="41"/>
@@ -5845,13 +5854,13 @@
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>157</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="T50" s="41"/>
       <c r="U50" s="41"/>
@@ -5875,10 +5884,10 @@
         <v>405</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="T51" s="41"/>
       <c r="U51" s="41"/>
@@ -5917,7 +5926,7 @@
         <v>183</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>232</v>
@@ -5926,10 +5935,10 @@
         <v>802</v>
       </c>
       <c r="N52" s="7" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="T52" s="41"/>
       <c r="U52" s="41"/>
@@ -6004,13 +6013,13 @@
         <v>675</v>
       </c>
       <c r="O54" s="13" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="P54" s="8" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="T54" s="41"/>
       <c r="U54" s="41"/>
@@ -6112,10 +6121,10 @@
         <v>195</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="P56" s="10" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="Q56" s="11" t="s">
         <v>658</v>
@@ -6154,19 +6163,19 @@
         <v>266</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>820</v>
+        <v>1012</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="T57" s="41"/>
       <c r="U57" s="41"/>
@@ -6202,13 +6211,13 @@
         <v>431</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="T58" s="41"/>
       <c r="U58" s="41"/>
@@ -6247,22 +6256,22 @@
         <v>230</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>820</v>
+        <v>1013</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="M59" s="12" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="T59" s="41"/>
       <c r="U59" s="41"/>
@@ -6283,7 +6292,7 @@
         <v>171</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>277</v>
@@ -6295,7 +6304,7 @@
         <v>175</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>816</v>
@@ -6304,10 +6313,10 @@
         <v>170</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>289</v>
@@ -6328,7 +6337,7 @@
         <v>161</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>192</v>
@@ -6337,7 +6346,7 @@
         <v>191</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="T61" s="41"/>
       <c r="U61" s="41"/>
@@ -6388,7 +6397,7 @@
         <v>818</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="P62" s="1" t="s">
         <v>177</v>
@@ -6469,7 +6478,7 @@
         <v>774</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="T64" s="41"/>
       <c r="U64" s="41"/>
@@ -6526,13 +6535,13 @@
         <v>232</v>
       </c>
       <c r="Q65" s="6" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="R65" s="7" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="T65" s="41"/>
       <c r="U65" s="41"/>
@@ -6583,16 +6592,16 @@
         <v>810</v>
       </c>
       <c r="O66" s="6" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P66" s="8" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="T66" s="41"/>
       <c r="U66" s="41"/>
@@ -6616,13 +6625,13 @@
         <v>224</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="T67" s="41"/>
       <c r="U67" s="41"/>
@@ -6691,7 +6700,7 @@
         <v>289</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="H69" s="11" t="s">
         <v>163</v>
@@ -6700,7 +6709,7 @@
         <v>556</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="T69" s="41"/>
       <c r="U69" s="41"/>
@@ -6724,19 +6733,19 @@
         <v>173</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="T70" s="41"/>
       <c r="U70" s="41"/>
@@ -6760,7 +6769,7 @@
         <v>191</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="T71" s="41"/>
       <c r="U71" s="41"/>
@@ -6811,7 +6820,7 @@
         <v>484</v>
       </c>
       <c r="O72" s="11" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="P72" s="11" t="s">
         <v>430</v>
@@ -6827,19 +6836,19 @@
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>896</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>898</v>
-      </c>
       <c r="E73" s="11" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="T73" s="41"/>
       <c r="U73" s="41"/>
@@ -6878,10 +6887,10 @@
         <v>276</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="M74" s="6" t="s">
         <v>335</v>
@@ -6890,7 +6899,7 @@
         <v>326</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="T74" s="41"/>
       <c r="U74" s="41"/>
@@ -6935,7 +6944,7 @@
         <v>224</v>
       </c>
       <c r="M75" s="6" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="N75" s="11" t="s">
         <v>373</v>
@@ -6944,16 +6953,16 @@
         <v>235</v>
       </c>
       <c r="P75" s="11" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="R75" s="1" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="S75" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="T75" s="41"/>
       <c r="U75" s="41"/>
@@ -7001,7 +7010,7 @@
         <v>431</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="O76" s="6" t="s">
         <v>335</v>
@@ -7010,13 +7019,13 @@
         <v>232</v>
       </c>
       <c r="Q76" s="7" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="R76" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="S76" s="1" t="s">
         <v>981</v>
-      </c>
-      <c r="S76" s="1" t="s">
-        <v>983</v>
       </c>
       <c r="T76" s="41"/>
       <c r="U76" s="41"/>
@@ -7040,7 +7049,7 @@
         <v>430</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="T77" s="41"/>
       <c r="U77" s="41"/>
@@ -7070,13 +7079,13 @@
         <v>429</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I78" s="12" t="s">
         <v>252</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="T78" s="41"/>
       <c r="U78" s="41"/>
@@ -7112,7 +7121,7 @@
         <v>272</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>162</v>
@@ -7121,10 +7130,10 @@
         <v>278</v>
       </c>
       <c r="M79" s="11" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="N79" s="8" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="T79" s="41"/>
       <c r="U79" s="41"/>
@@ -7166,13 +7175,13 @@
         <v>252</v>
       </c>
       <c r="L80" s="13" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="M80" s="13" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="N80" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="T80" s="41"/>
       <c r="U80" s="41"/>
@@ -7217,7 +7226,7 @@
         <v>274</v>
       </c>
       <c r="M81" s="8" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="N81" s="6" t="s">
         <v>429</v>
@@ -7229,16 +7238,16 @@
         <v>252</v>
       </c>
       <c r="Q81" s="8" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="R81" s="8" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="S81" s="9" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T81" s="41" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="U81" s="41"/>
       <c r="V81" s="41"/>
@@ -7279,7 +7288,7 @@
         <v>289</v>
       </c>
       <c r="L82" s="13" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="M82" s="13" t="s">
         <v>373</v>
@@ -7333,10 +7342,10 @@
         <v>335</v>
       </c>
       <c r="M83" s="8" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T83" s="41"/>
       <c r="U83" s="41"/>
@@ -7378,7 +7387,7 @@
         <v>240</v>
       </c>
       <c r="L84" s="11" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="T84" s="41"/>
       <c r="U84" s="41"/>
@@ -7432,13 +7441,13 @@
         <v>173</v>
       </c>
       <c r="P85" s="13" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="Q85" s="10" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="T85" s="41"/>
       <c r="U85" s="41"/>
@@ -7447,16 +7456,16 @@
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>157</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="T86" s="41"/>
       <c r="U86" s="41"/>
@@ -7510,7 +7519,7 @@
         <v>326</v>
       </c>
       <c r="P87" s="6" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="Q87" s="8" t="s">
         <v>313</v>
@@ -7519,16 +7528,16 @@
         <v>609</v>
       </c>
       <c r="S87" s="11" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="T87" s="44" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="U87" s="41" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="V87" s="41" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="W87" s="2" t="s">
         <v>307</v>
@@ -7569,7 +7578,7 @@
         <v>232</v>
       </c>
       <c r="L88" s="6" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M88" s="11" t="s">
         <v>805</v>
@@ -7620,16 +7629,16 @@
         <v>440</v>
       </c>
       <c r="N89" s="7" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="P89" s="7" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="T89" s="41"/>
       <c r="U89" s="41"/>
@@ -7638,13 +7647,13 @@
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>157</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>183</v>
@@ -7692,7 +7701,7 @@
         <v>252</v>
       </c>
       <c r="M91" s="6" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="N91" s="8" t="s">
         <v>276</v>
@@ -7740,7 +7749,7 @@
         <v>252</v>
       </c>
       <c r="M92" s="10" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="N92" s="8" t="s">
         <v>224</v>
@@ -7764,7 +7773,7 @@
         <v>558</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>388</v>
@@ -7779,13 +7788,13 @@
         <v>430</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="T93" s="41"/>
       <c r="U93" s="41"/>
@@ -7806,7 +7815,7 @@
         <v>170</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="F94" s="13" t="s">
         <v>430</v>
@@ -7815,10 +7824,10 @@
         <v>326</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="T94" s="41"/>
       <c r="U94" s="41"/>
@@ -7869,13 +7878,13 @@
         <v>431</v>
       </c>
       <c r="O95" s="11" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="P95" s="13" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="Q95" s="8" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="T95" s="41"/>
       <c r="U95" s="41"/>
@@ -7884,7 +7893,7 @@
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>157</v>
@@ -7932,10 +7941,10 @@
         <v>194</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T97" s="41"/>
       <c r="U97" s="41"/>
@@ -7977,13 +7986,13 @@
         <v>252</v>
       </c>
       <c r="L98" s="10" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="M98" s="10" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="T98" s="41"/>
       <c r="U98" s="41"/>
@@ -8070,13 +8079,13 @@
         <v>273</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M100" s="8" t="s">
         <v>170</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="T100" s="41"/>
       <c r="U100" s="41"/>
@@ -8100,7 +8109,7 @@
         <v>252</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="T101" s="41"/>
       <c r="U101" s="41"/>
@@ -8145,13 +8154,13 @@
         <v>313</v>
       </c>
       <c r="M102" s="6" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="N102" s="10" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="T102" s="41"/>
       <c r="U102" s="41"/>
@@ -8199,7 +8208,7 @@
         <v>326</v>
       </c>
       <c r="N103" s="10" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="T103" s="41"/>
       <c r="U103" s="41"/>
@@ -8229,19 +8238,19 @@
         <v>802</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="J104" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="K104" s="11" t="s">
         <v>924</v>
       </c>
-      <c r="K104" s="11" t="s">
-        <v>926</v>
-      </c>
       <c r="L104" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="T104" s="41"/>
       <c r="U104" s="41"/>
@@ -8262,7 +8271,7 @@
         <v>184</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F105" s="13" t="s">
         <v>307</v>
@@ -8274,7 +8283,7 @@
         <v>509</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="T105" s="41"/>
       <c r="U105" s="41"/>
@@ -8340,16 +8349,16 @@
         <v>278</v>
       </c>
       <c r="J107" s="6" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="K107" s="6" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="L107" s="9" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="M107" s="10" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="T107" s="41"/>
       <c r="U107" s="41"/>
@@ -8394,7 +8403,7 @@
         <v>240</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="T108" s="41"/>
       <c r="U108" s="41"/>
@@ -8421,7 +8430,7 @@
         <v>172</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="T109" s="41"/>
       <c r="U109" s="41"/>
@@ -8451,22 +8460,22 @@
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>157</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="T111" s="41"/>
       <c r="U111" s="41"/>
@@ -8520,7 +8529,7 @@
         <v>440</v>
       </c>
       <c r="P112" s="6" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="T112" s="41"/>
       <c r="U112" s="41"/>
@@ -8556,7 +8565,7 @@
         <v>802</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="T113" s="41"/>
       <c r="U113" s="41"/>
@@ -8580,7 +8589,7 @@
         <v>609</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>610</v>
@@ -8589,7 +8598,7 @@
         <v>169</v>
       </c>
       <c r="I114" s="10" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="J114" s="6" t="s">
         <v>440</v>
@@ -8601,7 +8610,7 @@
         <v>611</v>
       </c>
       <c r="M114" s="8" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="N114" s="9" t="s">
         <v>173</v>
@@ -8610,13 +8619,13 @@
         <v>802</v>
       </c>
       <c r="P114" s="11" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="Q114" s="9" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="R114" s="8" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="T114" s="41"/>
       <c r="U114" s="41"/>
@@ -8646,7 +8655,7 @@
         <v>252</v>
       </c>
       <c r="H115" s="13" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="T115" s="41"/>
       <c r="U115" s="41"/>
@@ -8691,7 +8700,7 @@
         <v>192</v>
       </c>
       <c r="M116" s="8" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="N116" s="11" t="s">
         <v>417</v>
@@ -8721,7 +8730,7 @@
         <v>232</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="T117" s="41"/>
       <c r="U117" s="41"/>
@@ -8787,7 +8796,7 @@
         <v>184</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>232</v>
@@ -8799,7 +8808,7 @@
         <v>500</v>
       </c>
       <c r="H119" s="9" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="I119" s="6" t="s">
         <v>326</v>
@@ -8808,7 +8817,7 @@
         <v>170</v>
       </c>
       <c r="K119" s="8" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="T119" s="41"/>
       <c r="U119" s="41"/>
@@ -8835,19 +8844,19 @@
         <v>808</v>
       </c>
       <c r="G120" s="10" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="J120" s="11" t="s">
         <v>170</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="T120" s="41"/>
       <c r="U120" s="41"/>
@@ -8868,7 +8877,7 @@
         <v>628</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="F121" s="11" t="s">
         <v>273</v>
@@ -8880,10 +8889,10 @@
         <v>173</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="J121" s="11" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="T121" s="41"/>
       <c r="U121" s="41"/>
@@ -8928,16 +8937,16 @@
         <v>806</v>
       </c>
       <c r="M122" s="11" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="N122" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="O122" s="13" t="s">
         <v>924</v>
       </c>
-      <c r="O122" s="13" t="s">
-        <v>926</v>
-      </c>
       <c r="P122" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="T122" s="41"/>
       <c r="U122" s="41"/>
@@ -8982,7 +8991,7 @@
         <v>774</v>
       </c>
       <c r="M123" s="7" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="T123" s="41"/>
       <c r="U123" s="41"/>
@@ -9009,7 +9018,7 @@
         <v>642</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="H124" s="13" t="s">
         <v>222</v>
@@ -9018,7 +9027,7 @@
         <v>313</v>
       </c>
       <c r="J124" s="8" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="T124" s="41"/>
       <c r="U124" s="41"/>
@@ -9066,7 +9075,7 @@
         <v>240</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="T125" s="41"/>
       <c r="U125" s="41"/>
@@ -9105,7 +9114,7 @@
         <v>232</v>
       </c>
       <c r="K126" s="8" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="T126" s="41"/>
       <c r="U126" s="41"/>
@@ -9156,22 +9165,22 @@
         <v>163</v>
       </c>
       <c r="O127" s="6" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="P127" s="6" t="s">
         <v>499</v>
       </c>
       <c r="Q127" s="6" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="R127" s="7" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="S127" s="9" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="T127" s="41" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="U127" s="41"/>
       <c r="V127" s="41"/>
@@ -9206,13 +9215,13 @@
     </row>
     <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B129" s="10" t="s">
         <v>157</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="T129" s="41"/>
       <c r="U129" s="41"/>
@@ -9260,10 +9269,10 @@
         <v>170</v>
       </c>
       <c r="N130" s="7" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="O130" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="P130" s="1" t="s">
         <v>162</v>
@@ -9314,19 +9323,19 @@
         <v>224</v>
       </c>
       <c r="N131" s="7" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="O131" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="P131" s="9" t="s">
         <v>173</v>
       </c>
       <c r="Q131" s="6" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="R131" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="T131" s="41"/>
       <c r="U131" s="41"/>
@@ -9359,13 +9368,13 @@
         <v>675</v>
       </c>
       <c r="I132" s="10" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="T132" s="41"/>
       <c r="U132" s="41"/>
@@ -9389,16 +9398,16 @@
         <v>183</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="G133" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="I133" s="13" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>289</v>
@@ -9443,7 +9452,7 @@
         <v>326</v>
       </c>
       <c r="L134" s="5" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="M134" s="9" t="s">
         <v>173</v>
@@ -9506,7 +9515,7 @@
         <v>170</v>
       </c>
       <c r="G136" s="9" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T136" s="41"/>
       <c r="U136" s="41"/>
@@ -9548,10 +9557,10 @@
         <v>232</v>
       </c>
       <c r="L137" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="M137" s="11" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="T137" s="41"/>
       <c r="U137" s="41"/>
@@ -9629,7 +9638,7 @@
         <v>173</v>
       </c>
       <c r="N139" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="O139" s="10" t="s">
         <v>432</v>
@@ -9653,7 +9662,7 @@
         <v>691</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E140" s="6" t="s">
         <v>161</v>
@@ -9671,7 +9680,7 @@
         <v>272</v>
       </c>
       <c r="J140" s="13" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="K140" s="11" t="s">
         <v>373</v>
@@ -9686,13 +9695,13 @@
         <v>817</v>
       </c>
       <c r="O140" s="8" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="P140" s="9" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="T140" s="41"/>
       <c r="U140" s="41"/>
@@ -9749,7 +9758,7 @@
         <v>173</v>
       </c>
       <c r="Q141" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="T141" s="41"/>
       <c r="U141" s="41"/>
@@ -9782,10 +9791,10 @@
         <v>260</v>
       </c>
       <c r="I142" s="9" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="T142" s="41"/>
       <c r="U142" s="41"/>
@@ -9854,7 +9863,7 @@
         <v>707</v>
       </c>
       <c r="E144" s="13" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F144" s="6" t="s">
         <v>328</v>
@@ -9941,7 +9950,7 @@
         <v>232</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="T145" s="41"/>
       <c r="U145" s="41"/>
@@ -9971,7 +9980,7 @@
         <v>720</v>
       </c>
       <c r="H146" s="10" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="T146" s="41"/>
       <c r="U146" s="41"/>
@@ -10001,7 +10010,7 @@
         <v>721</v>
       </c>
       <c r="H147" s="10" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="T147" s="41"/>
       <c r="U147" s="41"/>
@@ -10049,10 +10058,10 @@
         <v>232</v>
       </c>
       <c r="N148" s="6" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T148" s="41"/>
       <c r="U148" s="41"/>
@@ -10094,7 +10103,7 @@
         <v>432</v>
       </c>
       <c r="L149" s="10" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="M149" s="10" t="s">
         <v>173</v>
@@ -10106,13 +10115,13 @@
         <v>802</v>
       </c>
       <c r="P149" s="12" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="Q149" s="8" t="s">
         <v>440</v>
       </c>
       <c r="R149" s="8" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="T149" s="41"/>
       <c r="U149" s="41"/>
@@ -10163,13 +10172,13 @@
         <v>240</v>
       </c>
       <c r="O150" s="12" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="P150" s="13" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="Q150" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="T150" s="41"/>
       <c r="U150" s="41"/>
@@ -10199,7 +10208,7 @@
         <v>196</v>
       </c>
       <c r="H151" s="11" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="T151" s="41"/>
       <c r="U151" s="41"/>
@@ -10217,7 +10226,7 @@
         <v>440</v>
       </c>
       <c r="D152" s="11" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T152" s="41"/>
       <c r="U152" s="41"/>
@@ -10256,16 +10265,16 @@
         <v>339</v>
       </c>
       <c r="K153" s="9" t="s">
-        <v>820</v>
+        <v>1014</v>
       </c>
       <c r="L153" s="11" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="M153" s="6" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="T153" s="41"/>
       <c r="U153" s="41"/>
@@ -10286,16 +10295,16 @@
         <v>811</v>
       </c>
       <c r="E154" s="13" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F154" s="6" t="s">
         <v>595</v>
       </c>
       <c r="G154" s="13" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="T154" s="41"/>
       <c r="U154" s="41"/>
@@ -10328,7 +10337,7 @@
         <v>232</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="T155" s="41"/>
       <c r="U155" s="41"/>
@@ -10373,10 +10382,10 @@
         <v>746</v>
       </c>
       <c r="M156" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="N156" s="10" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="T156" s="41"/>
       <c r="U156" s="41"/>
@@ -10412,10 +10421,10 @@
         <v>819</v>
       </c>
       <c r="J157" s="8" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="K157" s="6" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="T157" s="41"/>
       <c r="U157" s="41"/>
@@ -10466,13 +10475,13 @@
         <v>805</v>
       </c>
       <c r="O158" s="11" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="P158" s="6" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q158" s="1" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="T158" s="41"/>
       <c r="U158" s="41"/>
@@ -10541,19 +10550,19 @@
         <v>807</v>
       </c>
       <c r="I160" s="8" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J160" s="8" t="s">
         <v>278</v>
       </c>
       <c r="K160" s="7" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="L160" s="7" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="M160" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="T160" s="41"/>
       <c r="U160" s="41"/>
@@ -10589,7 +10598,7 @@
         <v>240</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="T161" s="41"/>
       <c r="U161" s="41"/>
@@ -10667,7 +10676,7 @@
         <v>184</v>
       </c>
       <c r="J163" s="10" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="K163" s="7" t="s">
         <v>173</v>
@@ -10679,22 +10688,22 @@
         <v>815</v>
       </c>
       <c r="N163" s="6" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="O163" s="6" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="P163" s="10" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="Q163" s="8" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="R163" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="S163" s="1" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="T163" s="41"/>
       <c r="U163" s="41"/>
@@ -10718,22 +10727,22 @@
         <v>440</v>
       </c>
       <c r="F164" s="13" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="G164" s="10" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="H164" s="9" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="I164" s="9" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="J164" s="1" t="s">
         <v>232</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="T164" s="41"/>
       <c r="U164" s="41"/>
@@ -10796,16 +10805,16 @@
         <v>326</v>
       </c>
       <c r="G166" s="13" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="H166" s="13" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="T166" s="41"/>
       <c r="U166" s="41"/>
@@ -10832,10 +10841,10 @@
         <v>481</v>
       </c>
       <c r="G167" s="10" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="T167" s="41"/>
       <c r="U167" s="41"/>
@@ -10859,7 +10868,7 @@
         <v>183</v>
       </c>
       <c r="F168" s="7" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="G168" s="10" t="s">
         <v>458</v>
@@ -10871,16 +10880,16 @@
         <v>339</v>
       </c>
       <c r="J168" s="6" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="K168" s="9" t="s">
         <v>335</v>
       </c>
       <c r="L168" s="10" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="M168" s="8" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="N168" s="1" t="s">
         <v>161</v>
@@ -10892,7 +10901,7 @@
     </row>
     <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B169" s="10" t="s">
         <v>157</v>
@@ -10901,16 +10910,16 @@
         <v>677</v>
       </c>
       <c r="D169" s="13" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E169" s="9" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="T169" s="41"/>
       <c r="U169" s="41"/>
@@ -10952,10 +10961,10 @@
         <v>194</v>
       </c>
       <c r="L170" s="11" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="M170" s="12" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="T170" s="41"/>
       <c r="U170" s="41"/>
@@ -10988,7 +10997,7 @@
         <v>265</v>
       </c>
       <c r="I171" s="9" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="T171" s="41"/>
       <c r="U171" s="41"/>
@@ -11015,13 +11024,13 @@
         <v>483</v>
       </c>
       <c r="G172" s="9" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="H172" s="10" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="I172" s="10" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J172" s="1" t="s">
         <v>289</v>
@@ -11054,7 +11063,7 @@
         <v>276</v>
       </c>
       <c r="H173" s="18" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="I173" s="36" t="s">
         <v>675</v>
@@ -11063,10 +11072,10 @@
         <v>806</v>
       </c>
       <c r="K173" s="18" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="L173" s="16" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="M173" s="3" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
Soul Fighter Lux and link updates
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="1020">
   <si>
     <t>Aatrox</t>
   </si>
@@ -3788,8 +3788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="L61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T85" sqref="T85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7279,10 +7279,12 @@
       <c r="S81" s="9" t="s">
         <v>895</v>
       </c>
-      <c r="T81" s="41" t="s">
+      <c r="T81" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="U81" s="41" t="s">
         <v>908</v>
       </c>
-      <c r="U81" s="41"/>
       <c r="V81" s="41"/>
       <c r="W81" s="2"/>
     </row>

</xml_diff>

<commit_message>
Patch 15.07 und 15.08
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="1033">
   <si>
     <t>Aatrox</t>
   </si>
@@ -3099,6 +3099,30 @@
   </si>
   <si>
     <t>Grand Reckoning</t>
+  </si>
+  <si>
+    <t>Urgot the Clogfather</t>
+  </si>
+  <si>
+    <t>Grill Master</t>
+  </si>
+  <si>
+    <t>Pengu</t>
+  </si>
+  <si>
+    <t>Glizzy</t>
+  </si>
+  <si>
+    <t>Cat-in-the-Box</t>
+  </si>
+  <si>
+    <t>Sahn-Uzal</t>
+  </si>
+  <si>
+    <t>Fatebreaker</t>
+  </si>
+  <si>
+    <t>Fatemaker</t>
   </si>
 </sst>
 </file>
@@ -3803,8 +3827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" topLeftCell="G79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P93" sqref="P93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4695,6 +4719,9 @@
       <c r="I23" s="11" t="s">
         <v>273</v>
       </c>
+      <c r="J23" s="1" t="s">
+        <v>1026</v>
+      </c>
       <c r="T23" s="41"/>
       <c r="U23" s="41"/>
       <c r="V23" s="41"/>
@@ -5643,6 +5670,9 @@
       </c>
       <c r="Q43" s="1" t="s">
         <v>986</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>1027</v>
       </c>
       <c r="T43" s="41"/>
       <c r="U43" s="41"/>
@@ -7364,6 +7394,9 @@
       <c r="O82" s="6" t="s">
         <v>556</v>
       </c>
+      <c r="P82" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="T82" s="41"/>
       <c r="U82" s="41"/>
       <c r="V82" s="41"/>
@@ -7411,6 +7444,9 @@
       </c>
       <c r="N83" s="1" t="s">
         <v>895</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>1031</v>
       </c>
       <c r="T83" s="41"/>
       <c r="U83" s="41"/>
@@ -7677,6 +7713,9 @@
       <c r="M89" s="11" t="s">
         <v>805</v>
       </c>
+      <c r="N89" s="1" t="s">
+        <v>1030</v>
+      </c>
       <c r="T89" s="41"/>
       <c r="U89" s="41"/>
       <c r="V89" s="41"/>
@@ -7752,6 +7791,9 @@
       <c r="D91" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="E91" s="1" t="s">
+        <v>1028</v>
+      </c>
       <c r="T91" s="41"/>
       <c r="U91" s="41"/>
       <c r="V91" s="41"/>
@@ -7851,6 +7893,9 @@
       <c r="N93" s="8" t="s">
         <v>224</v>
       </c>
+      <c r="O93" s="1" t="s">
+        <v>1032</v>
+      </c>
       <c r="T93" s="41"/>
       <c r="U93" s="41"/>
       <c r="V93" s="41"/>
@@ -9066,6 +9111,9 @@
       <c r="P123" s="1" t="s">
         <v>891</v>
       </c>
+      <c r="Q123" s="1" t="s">
+        <v>1029</v>
+      </c>
       <c r="T123" s="41"/>
       <c r="U123" s="41"/>
       <c r="V123" s="41"/>
@@ -9722,6 +9770,9 @@
       <c r="H139" s="12" t="s">
         <v>252</v>
       </c>
+      <c r="I139" s="1" t="s">
+        <v>1031</v>
+      </c>
       <c r="T139" s="41"/>
       <c r="U139" s="41"/>
       <c r="V139" s="41"/>
@@ -10031,6 +10082,9 @@
       <c r="Q145" s="12" t="s">
         <v>252</v>
       </c>
+      <c r="R145" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="T145" s="41"/>
       <c r="U145" s="41"/>
       <c r="V145" s="41"/>
@@ -10141,6 +10195,9 @@
       </c>
       <c r="H148" s="10" t="s">
         <v>891</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>1025</v>
       </c>
       <c r="T148" s="41"/>
       <c r="U148" s="41"/>

</xml_diff>

<commit_message>
Xin Zhao visual update
</commit_message>
<xml_diff>
--- a/src/assets/resources/Tierlist.xlsx
+++ b/src/assets/resources/Tierlist.xlsx
@@ -3869,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P80" sqref="P80"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F163" sqref="F163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10960,19 +10960,19 @@
       <c r="A163" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B163" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C163" s="11" t="s">
+      <c r="B163" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="C163" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="D163" s="11" t="s">
+      <c r="D163" s="45" t="s">
         <v>507</v>
       </c>
       <c r="E163" s="10" t="s">
         <v>766</v>
       </c>
-      <c r="F163" s="8" t="s">
+      <c r="F163" s="45" t="s">
         <v>767</v>
       </c>
       <c r="G163" s="6" t="s">

</xml_diff>